<commit_message>
Task updated on 03-07-2025
</commit_message>
<xml_diff>
--- a/Scripts/output/patents_details.xlsx
+++ b/Scripts/output/patents_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Code\Scripts\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467830EB-97A6-4D41-AC38-784B99750712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C138C38-BAB6-4DE8-8106-88A8CFE1083D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="6456" yWindow="4416" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,53 +61,6 @@
     <t>Cleaned Claims</t>
   </si>
   <si>
-    <t>EP3589834A1</t>
-  </si>
-  <si>
-    <t>EP18761706.3A</t>
-  </si>
-  <si>
-    <t>A starter system for a vehicle</t>
-  </si>
-  <si>
-    <t>The present subject matter provides a starter system (200) for a vehicle (100). The starter system (200) includes a starter means (125E) functionally 5 connected to a crankshaft (125B) of a power unit (125, 425). A starter control unit (210) initially enabling cranking of the power unit (125, 425) through the starter means (125E) at a first speed. Then the starter control unit (210) checks for at least a first parameter of the power unit (125, 425). Subsequently, the starter control unit (210) depending on the first parameter enables cranking of the power 10 unit (125, 425) at a second speed. The second speed is greater than the first speed. The starter system (200) of the present subject matter improves startability and also reduces power consumption of power source (205) driving the starter means (125E).</t>
-  </si>
-  <si>
-    <t>2020-01-08</t>
-  </si>
-  <si>
-    <t>Vaidyanathan HEMAVATHY, Thalakku PANDIAN MANIKANDAN, Arumugham SIVAKUMAR, Davinder KUMAR</t>
-  </si>
-  <si>
-    <t>Claim 1: 1. A starter system (200, 201) for a vehicle (100), said starter system (200, 201) comprising: 
-       a starter means (125E) functionally connected to a crankshaft (125B) of a power unit (125, 425) of said vehicle (100); 
-       a power source (205) electrically coupled to said starter means (125E) for driving said starter means (125E); and 
-       a starter control unit (210), said starter control unit (210) initially enables cranking of said power unit (125, 425) through said starter means (125E) at a first speed, said starter control unit (210) checks for at least a first parameter of said power unit (125, 425), and subsequently said starter control unit (210) depending on said first parameter enables cranking of said power unit (125, 425) at a second speed, wherein said second speed being greater than said first speed.
-Claim 2: 2. The starter system (200, 201) as claimed in claim 1, wherein said first parameter includes at least one of an engine speed, and rotational speed of crankshaft (125B) or rotational speed of one of more rotating members connected to said crankshaft (125B).
-Claim 3: 3. The starter system (200, 201) as claimed in claim 1, wherein said starter means (125E) includes a rotor (125ER), and said rotor (125ER) is mounted to at least one of said crankshaft (125B) or a shaft disposed substantially parallel to said crankshaft (125B)..
-Claim 4: 4. The starter system (200, 201) as claimed in claim 1, wherein said starter means (125E) includes an integrated starter generator (125E), a magneto, or an electric motor, wherein said integrated starter generator (125E) includes a stator (125ES) and a rotor (125ER), said rotor (125ER) functionally connected to said 
- crankshaft (125B) and said rotor comprising plurality of magnetic members, and said stator (125ES) supported by said power unit (125).
-Claim 5: 5. The starter system (200, 201) as claimed in claim 1, wherein said starter control unit (210) is capable of rotating said crankshaft (125B) in a reverse rotation so that a piston of the power unit (125, 425) is positioned in a start position of an expansion stroke thereof.
-Claim 6: 6. The starter system (200, 201) as claimed in claim 1, wherein said starter control unit (210) compares said first parameter being an engine speed, during every crank attempt, with a second pre-determined speed, &amp; starter control unit (210) identifies a malfunction when said first speed is equal to or greater than said second-predetermined speed.
-Claim 7: 7. The starter system (201) as claimed in claim 1 , wherein said starter system (201) disposed substantially separately from said power unit (425), wherein a drive pulley (410) connected to the rotor (125ER) of the starter means (125E) and a driven pulley (415) connected to the crankshaft (125B), and a belt drive (405) connecting the drive pulley (410) with the driven pulley (415) whereby said the driven pulley (415) is adapted to act as a flywheel for the power unit (425).
-Claim 8: 8. The starter system (200, 201) as claimed in claim 1 , wherein said first speed is incremented to said second speed by at least one of progressive increment, exponential increment, and random increment.
-Claim 9: 9. The starter system (200, 201) as claimed in claim 1, wherein said starter control unit (210) includes plurality of Metal oxide semiconductor field effect transistors (Ml , M2, M3, M4, M5, and M6) that are electrically coupled to a winding(s) of said stator (125ES), and plurality of Metal oxide semiconductor field effect transistors (Ml , M2, M3, M4, M5, and M6) driven by a microcontroller (210E) of said starter control unit (210), and said windings are connected at least by one of star or delta connection.
-Claim 10: 10. The starter system (200, 201) as claimed in claim 1, wherein vehicle (100) includes at least one of a two- wheeled vehicle (100) or a three-wheeled vehicle.
-Claim 11: 11. A method of starting a power unit (125, 425) through a starter system (200, 201), said power unit (125, 425) includes a crankshaft (125B) operatively connected to a starter means (125E), said method comprising the steps of: 
-       enabling said starter means (125E) to crank said power unit (125, 425) at a first speed by a starter control unit (210) of said starter system (200, 201); checking for a first parameter of said power unit (125, 425) by said starter control, unit (210); and 
-       subsequently depending on said first parameter enabling cranking of said power unit (125, 425) at a second speed by said starter means (125E), wherein said second speed being greater than said first speed.
-Claim 12: 12. The method of starting a power unit (125, 425) as claimed in claim 9 further comprises comparing, during every crank attempt, said first speed with a second pre-determined speed, and activating a malfunction signal when said first speed is equal to or greater than said second-predetermined speed.</t>
-  </si>
-  <si>
-    <t>present subject matter provides starter system 200 for vehicle 100 starter system 200 includes starter means 125e functionally 5 connected crankshaft 125b power unit 125 425 starter control unit 210 initially enabling cranking power unit 125 425 through starter means 125e at first speed then starter control unit 210 checks for at least first parameter power unit 125 425 subsequently starter control unit 210 depending on first parameter enables cranking power 10 unit 125 425 at second speed second speed is greater than first speed starter system 200 present subject matter improves startability also reduces power consumption power source 205 driving starter means 125e</t>
-  </si>
-  <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>1 1 starter system 200 201 for vehicle 100 starter system 200 201 comprising starter means 125e functionally connected crankshaft 125b power unit 125 425 vehicle 100 power source 205 electrically coupled starter means 125e for driving starter means 125e starter control unit 210 starter control unit 210 initially enables cranking power unit 125 425 through starter means 125e at first speed starter control unit 210 checks for at least first parameter power unit 125 425 subsequently starter control unit 210 depending on first parameter enables cranking power unit 125 425 at second speed second speed being greater than first speed 2 2 starter system 200 201 as claimed 1 first parameter includes at least one engine speed rotational speed crankshaft 125b rotational speed one more rotating members connected crankshaft 125b 3 3 starter system 200 201 as claimed 1 starter means 125e includes rotor 125er rotor 125er is mounted at least one crankshaft 125b shaft disposed substantially parallel crankshaft 125b 4 4 starter system 200 201 as claimed 1 starter means 125e includes integrated starter generator 125e magneto electric motor integrated starter generator 125e includes stator 125es rotor 125er rotor 125er functionally connected crankshaft 125b rotor comprising plurality magnetic members stator 125es supported by power unit 125 5 5 starter system 200 201 as claimed 1 starter control unit 210 is capable rotating crankshaft 125b reverse rotation so that piston power unit 125 425 is positioned start position expansion stroke 6 6 starter system 200 201 as claimed 1 starter control unit 210 compares first parameter being engine speed during every crank attempt with second predetermined speed starter control unit 210 identifies malfunction when first speed is equal greater than secondpredetermined speed 7 7 starter system 201 as claimed 1 starter system 201 disposed substantially separately from power unit 425 drive pulley 410 connected rotor 125er starter means 125e driven pulley 415 connected crankshaft 125b belt drive 405 connecting drive pulley 410 with driven pulley 415 whereby driven pulley 415 is adapted act as flywheel for power unit 425 8 8 starter system 200 201 as claimed 1 first speed is incremented second speed by at least one progressive increment exponential increment random increment 9 9 starter system 200 201 as claimed 1 starter control unit 210 includes plurality metal oxide semiconductor field effect transistors ml m2 m3 m4 m5 m6 that are electrically coupled windings stator 125es plurality metal oxide semiconductor field effect transistors ml m2 m3 m4 m5 m6 driven by microcontroller 210e starter control unit 210 windings are connected at least by one star delta connection 10 10 starter system 200 201 as claimed 1 vehicle 100 includes at least one two wheeled vehicle 100 threewheeled vehicle 11 11 method starting power unit 125 425 through starter system 200 201 power unit 125 425 includes crankshaft 125b operatively connected starter means 125e method comprising steps enabling starter means 125e crank power unit 125 425 at first speed by starter control unit 210 starter system 200 201 checking for first parameter power unit 125 425 by starter control unit 210 subsequently depending on first parameter enabling cranking power unit 125 425 at second speed by starter means 125e second speed being greater than first speed 12 12 method starting power unit 125 425 as claimed 9 further comprises comparing during every crank attempt first speed with second predetermined speed activating malfunction signal when first speed is equal greater than secondpredetermined speed</t>
-  </si>
-  <si>
     <t>AU2012367784A1</t>
   </si>
   <si>
@@ -141,6 +94,9 @@
   </si>
   <si>
     <t>present subject matter discloses electrically operated clutch actuator for automatic transmission system for automatic disengagement controlled reengagement multi plate clutch assembly four stroke single cylinder internal combustion engine it comprises clutch actuation motor mounted external surface clutch cover sealed against ingress oil reduction gear box connected actuation motor for reducing power received from clutch actuation motor power transmission mechanism for converting rotational driving force clutch actuation motor into linear contact displacement force clutch actuation sensor for detecting actuation clutch invention increases operator comfort provides better rideability vehicle</t>
+  </si>
+  <si>
+    <t>na</t>
   </si>
   <si>
     <t>1 1 electrically operated clutch actuator system for internal combustion engine for actuating operation engagement disengagement 5 clutch comprising clutch actuation motor mounted external surface clutch cover sealed against ingress oil reduction gear box connected actuation motor for reducing power received from clutch actuation motor power transmission mechanism for converting rotational driving force clutch actuation motor into 10 linear contact displacement force clutch actuation sensor for detecting actuation clutch 2 2 clutch actuator system as claimed 1 power transmission mechanism comprises worm wheel actuator plunger having raised lug provided with extended shaft set caged 15 ramp balls return spring worm wheel actuator having multiple circumferential grooves on one their surfaces facing each other such way that set caged ramp balls is capable rotate between worm wheel actuator through circumferential grooves 20 3 3 clutch actuator system as claimed 1 reduction gear box comprises worm gear connecting reduction gear box worm wheel power transmission mechanism 4 4 clutch actuator system as claimed 1 power 25 transmission mechanism is mounted inside clutch cover 5 5 clutch actuation system as claimed any one preceding return spring is secured inner surface clutch cover so that return spring restricts rotational movement actuator allows only linear movement raised lug 30 actuator 11 wo 2013111154 pctin2012000852 6 6 clutch actuator system as claimed any preceding entry for worm gear motor shaft is provided on clutch cover 7 7 clutch actuator system as claimed any preceding s actuation motor may be supported on clutch cover either horizontally vertically through predetermined angle 8 8 internal combustion engine any type including horizontal internal combustion engine comprising clutch actuator system as claimed any preceding 10 9 9 clutch actuator system for internal combustion engine substantially as herein described illustrated with reference accompanying drawings 12</t>
@@ -639,9 +595,6 @@
     <t>Melkote Viraraghavachar NARASIMHAN, Varadha Iyengar LAKSHMINARASIMHAN, Varadarajan Ranganathan RAJAGOPALAN, K Kumar, Vythilingam KARUNAHARAN</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Claim 1: An internal combustion engine (100) comprising: 
        at least one port (132, 134); 
        a valve (164, 166) provided at the port (132, 134) to regulate an opening and closing of the port (132, 134); 
@@ -663,6 +616,53 @@
   </si>
   <si>
     <t>1 internal combustion engine 100 comprising at least one port 132 134 valve 164 166 provided at port 132 134 regulate opening closing port 132 134 valve seat 202 302 provided at port 132 134 for resting valve 164 166 valve seat rim 204 304 provided at valve seat 202 302 delay opening advance closing port 132 134 internal combustion engine 100 as claimed 1 valve seat rim 204 304 is provided at ircumference valve seat 202 302 valve seat rim 204 304 is cylindrical extending along longitudinal axis valve 164 166 internal combustion engine 100 as claimed 1 valve seat rim 204 304 extends length about 5 about 40 valve lift internal combustion engine 100 as claimed 1 valve seat rim 204 304 extends length about 1 millimeter 15 millimeter measured from valve seat 202 302 internal combustion engine 100 as claimed 1 valve seat rim 204 304 is provided at least at one inlet valve seat 202 exhaust valve seat 204 internal combustion engine 100 as claimed 1 inlet valve 164 opens inlet port 132 internal combustion engine 100 induct charge at about 240 290 degr s rotation crankshaft 104 from top dead centre tdc position closes inlet port 132 at about 280 330 degrees rotation crankshaft 104 from tdc position internal combustion engine 100 as claimed 1 exhaust valve 166 opens exhaust port 134 internal combustion engine 100 discharge combustion products at about 1 10 140 degrees rotation crankshaft 104 from top dead centre tdc position closes exhaust port 134 at about 240 280 degrees rotation crankshaft 104 from tdc position 8 internal combustion engine 100 as claimed 1 further comprising ignition element 138 ignite charge fires at about 325 360 degrees rotation crankshaft from tdc position 9 internal combustion engine 100 as claimed 1 expansion stroke internal combustion engine 100 begins at about 10 degrees rotation crankshaft 104 from top dead centre tdc position concludes at about 120 140 degrees rotation crankshaft 104 from tdc position 10 internal combustion engine 100 as claimed 1 expansion stroke takes place for about 1 10 150 degrees rotation crankshaft 104 compression stroke takes place for about 60 1 10 degrees rotation crankshaft 104 1 1 internal combustion engine 100 as claimed 1 piston 112 uncovers plurality transfer ports 116 cylinder wall 118 induct scavenging fluid at about 130 150 degrees rotation crankshaft 104 from top dead centre tdc positicn covers plurality transfer ports 116 at about 210 230 degrees rotation crankshaft 104 from tdc position</t>
+  </si>
+  <si>
+    <t>EP3589834A1</t>
+  </si>
+  <si>
+    <t>EP18761706.3A</t>
+  </si>
+  <si>
+    <t>A starter system for a vehicle</t>
+  </si>
+  <si>
+    <t>The present subject matter provides a starter system (200) for a vehicle (100). The starter system (200) includes a starter means (125E) functionally 5 connected to a crankshaft (125B) of a power unit (125, 425). A starter control unit (210) initially enabling cranking of the power unit (125, 425) through the starter means (125E) at a first speed. Then the starter control unit (210) checks for at least a first parameter of the power unit (125, 425). Subsequently, the starter control unit (210) depending on the first parameter enables cranking of the power 10 unit (125, 425) at a second speed. The second speed is greater than the first speed. The starter system (200) of the present subject matter improves startability and also reduces power consumption of power source (205) driving the starter means (125E).</t>
+  </si>
+  <si>
+    <t>2020-01-08</t>
+  </si>
+  <si>
+    <t>Vaidyanathan HEMAVATHY, Thalakku PANDIAN MANIKANDAN, Arumugham SIVAKUMAR, Davinder KUMAR</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Claim 1: 1. A starter system (200, 201) for a vehicle (100), said starter system (200, 201) comprising: 
+       a starter means (125E) functionally connected to a crankshaft (125B) of a power unit (125, 425) of said vehicle (100); 
+       a power source (205) electrically coupled to said starter means (125E) for driving said starter means (125E); and 
+       a starter control unit (210), said starter control unit (210) initially enables cranking of said power unit (125, 425) through said starter means (125E) at a first speed, said starter control unit (210) checks for at least a first parameter of said power unit (125, 425), and subsequently said starter control unit (210) depending on said first parameter enables cranking of said power unit (125, 425) at a second speed, wherein said second speed being greater than said first speed.
+Claim 2: 2. The starter system (200, 201) as claimed in claim 1, wherein said first parameter includes at least one of an engine speed, and rotational speed of crankshaft (125B) or rotational speed of one of more rotating members connected to said crankshaft (125B).
+Claim 3: 3. The starter system (200, 201) as claimed in claim 1, wherein said starter means (125E) includes a rotor (125ER), and said rotor (125ER) is mounted to at least one of said crankshaft (125B) or a shaft disposed substantially parallel to said crankshaft (125B)..
+Claim 4: 4. The starter system (200, 201) as claimed in claim 1, wherein said starter means (125E) includes an integrated starter generator (125E), a magneto, or an electric motor, wherein said integrated starter generator (125E) includes a stator (125ES) and a rotor (125ER), said rotor (125ER) functionally connected to said 
+ crankshaft (125B) and said rotor comprising plurality of magnetic members, and said stator (125ES) supported by said power unit (125).
+Claim 5: 5. The starter system (200, 201) as claimed in claim 1, wherein said starter control unit (210) is capable of rotating said crankshaft (125B) in a reverse rotation so that a piston of the power unit (125, 425) is positioned in a start position of an expansion stroke thereof.
+Claim 6: 6. The starter system (200, 201) as claimed in claim 1, wherein said starter control unit (210) compares said first parameter being an engine speed, during every crank attempt, with a second pre-determined speed, &amp; starter control unit (210) identifies a malfunction when said first speed is equal to or greater than said second-predetermined speed.
+Claim 7: 7. The starter system (201) as claimed in claim 1 , wherein said starter system (201) disposed substantially separately from said power unit (425), wherein a drive pulley (410) connected to the rotor (125ER) of the starter means (125E) and a driven pulley (415) connected to the crankshaft (125B), and a belt drive (405) connecting the drive pulley (410) with the driven pulley (415) whereby said the driven pulley (415) is adapted to act as a flywheel for the power unit (425).
+Claim 8: 8. The starter system (200, 201) as claimed in claim 1 , wherein said first speed is incremented to said second speed by at least one of progressive increment, exponential increment, and random increment.
+Claim 9: 9. The starter system (200, 201) as claimed in claim 1, wherein said starter control unit (210) includes plurality of Metal oxide semiconductor field effect transistors (Ml , M2, M3, M4, M5, and M6) that are electrically coupled to a winding(s) of said stator (125ES), and plurality of Metal oxide semiconductor field effect transistors (Ml , M2, M3, M4, M5, and M6) driven by a microcontroller (210E) of said starter control unit (210), and said windings are connected at least by one of star or delta connection.
+Claim 10: 10. The starter system (200, 201) as claimed in claim 1, wherein vehicle (100) includes at least one of a two- wheeled vehicle (100) or a three-wheeled vehicle.
+Claim 11: 11. A method of starting a power unit (125, 425) through a starter system (200, 201), said power unit (125, 425) includes a crankshaft (125B) operatively connected to a starter means (125E), said method comprising the steps of: 
+       enabling said starter means (125E) to crank said power unit (125, 425) at a first speed by a starter control unit (210) of said starter system (200, 201); checking for a first parameter of said power unit (125, 425) by said starter control, unit (210); and 
+       subsequently depending on said first parameter enabling cranking of said power unit (125, 425) at a second speed by said starter means (125E), wherein said second speed being greater than said first speed.
+Claim 12: 12. The method of starting a power unit (125, 425) as claimed in claim 9 further comprises comparing, during every crank attempt, said first speed with a second pre-determined speed, and activating a malfunction signal when said first speed is equal to or greater than said second-predetermined speed.</t>
+  </si>
+  <si>
+    <t>present subject matter provides starter system 200 for vehicle 100 starter system 200 includes starter means 125e functionally 5 connected crankshaft 125b power unit 125 425 starter control unit 210 initially enabling cranking power unit 125 425 through starter means 125e at first speed then starter control unit 210 checks for at least first parameter power unit 125 425 subsequently starter control unit 210 depending on first parameter enables cranking power 10 unit 125 425 at second speed second speed is greater than first speed starter system 200 present subject matter improves startability also reduces power consumption power source 205 driving starter means 125e</t>
+  </si>
+  <si>
+    <t>1 1 starter system 200 201 for vehicle 100 starter system 200 201 comprising starter means 125e functionally connected crankshaft 125b power unit 125 425 vehicle 100 power source 205 electrically coupled starter means 125e for driving starter means 125e starter control unit 210 starter control unit 210 initially enables cranking power unit 125 425 through starter means 125e at first speed starter control unit 210 checks for at least first parameter power unit 125 425 subsequently starter control unit 210 depending on first parameter enables cranking power unit 125 425 at second speed second speed being greater than first speed 2 2 starter system 200 201 as claimed 1 first parameter includes at least one engine speed rotational speed crankshaft 125b rotational speed one more rotating members connected crankshaft 125b 3 3 starter system 200 201 as claimed 1 starter means 125e includes rotor 125er rotor 125er is mounted at least one crankshaft 125b shaft disposed substantially parallel crankshaft 125b 4 4 starter system 200 201 as claimed 1 starter means 125e includes integrated starter generator 125e magneto electric motor integrated starter generator 125e includes stator 125es rotor 125er rotor 125er functionally connected crankshaft 125b rotor comprising plurality magnetic members stator 125es supported by power unit 125 5 5 starter system 200 201 as claimed 1 starter control unit 210 is capable rotating crankshaft 125b reverse rotation so that piston power unit 125 425 is positioned start position expansion stroke 6 6 starter system 200 201 as claimed 1 starter control unit 210 compares first parameter being engine speed during every crank attempt with second predetermined speed starter control unit 210 identifies malfunction when first speed is equal greater than secondpredetermined speed 7 7 starter system 201 as claimed 1 starter system 201 disposed substantially separately from power unit 425 drive pulley 410 connected rotor 125er starter means 125e driven pulley 415 connected crankshaft 125b belt drive 405 connecting drive pulley 410 with driven pulley 415 whereby driven pulley 415 is adapted act as flywheel for power unit 425 8 8 starter system 200 201 as claimed 1 first speed is incremented second speed by at least one progressive increment exponential increment random increment 9 9 starter system 200 201 as claimed 1 starter control unit 210 includes plurality metal oxide semiconductor field effect transistors ml m2 m3 m4 m5 m6 that are electrically coupled windings stator 125es plurality metal oxide semiconductor field effect transistors ml m2 m3 m4 m5 m6 driven by microcontroller 210e starter control unit 210 windings are connected at least by one star delta connection 10 10 starter system 200 201 as claimed 1 vehicle 100 includes at least one two wheeled vehicle 100 threewheeled vehicle 11 11 method starting power unit 125 425 through starter system 200 201 power unit 125 425 includes crankshaft 125b operatively connected starter means 125e method comprising steps enabling starter means 125e crank power unit 125 425 at first speed by starter control unit 210 starter system 200 201 checking for first parameter power unit 125 425 by starter control unit 210 subsequently depending on first parameter enabling cranking power unit 125 425 at second speed by starter means 125e second speed being greater than first speed 12 12 method starting power unit 125 425 as claimed 9 further comprises comparing during every crank attempt first speed with second predetermined speed activating malfunction signal when first speed is equal greater than secondpredetermined speed</t>
   </si>
 </sst>
 </file>
@@ -1030,22 +1030,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:M14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
-    <col min="9" max="9" width="26.21875" customWidth="1"/>
-    <col min="10" max="10" width="20.5546875" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" customWidth="1"/>
-    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.21875" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -1108,44 +1100,44 @@
       <c r="F2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
         <v>30</v>
@@ -1155,7 +1147,7 @@
         <v>31</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>32</v>
@@ -1190,7 +1182,7 @@
         <v>40</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>41</v>
@@ -1215,44 +1207,44 @@
       <c r="F5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
         <v>58</v>
@@ -1262,7 +1254,7 @@
         <v>59</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>60</v>
@@ -1297,7 +1289,7 @@
         <v>68</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>69</v>
@@ -1332,7 +1324,7 @@
         <v>77</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>78</v>
@@ -1367,7 +1359,7 @@
         <v>86</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>87</v>
@@ -1392,31 +1384,33 @@
       <c r="F10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>100</v>
@@ -1427,74 +1421,72 @@
       <c r="F11" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>119</v>
@@ -1509,7 +1501,7 @@
         <v>121</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>122</v>
@@ -1550,7 +1542,7 @@
         <v>131</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>132</v>

</xml_diff>